<commit_message>
added another expense - brad nailer
</commit_message>
<xml_diff>
--- a/expenses/expenses.xlsx
+++ b/expenses/expenses.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>Resistors, rotary encoder, buttons</t>
+  </si>
+  <si>
+    <t>first sheet of plywood</t>
+  </si>
+  <si>
+    <t>Home Depot</t>
+  </si>
+  <si>
+    <t>more LEDs and more power supplies</t>
+  </si>
+  <si>
+    <t>Brad Nailer and brads and pneumatic regulator</t>
+  </si>
+  <si>
+    <t>receipt filed?</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>more rotary encoders</t>
   </si>
 </sst>
 </file>
@@ -155,7 +176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -175,8 +196,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -186,8 +209,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -197,6 +229,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -206,6 +239,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -547,9 +581,10 @@
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="43" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -562,8 +597,11 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickTop="1">
+      <c r="E1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickTop="1">
       <c r="A2" s="1">
         <v>42348</v>
       </c>
@@ -576,8 +614,11 @@
       <c r="D2" s="2">
         <v>18.920000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>42377</v>
       </c>
@@ -590,8 +631,11 @@
       <c r="D3" s="2">
         <v>25.83</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>42393</v>
       </c>
@@ -604,8 +648,11 @@
       <c r="D4" s="2">
         <v>13.03</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>42403</v>
       </c>
@@ -618,8 +665,11 @@
       <c r="D5" s="2">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>42406</v>
       </c>
@@ -632,8 +682,11 @@
       <c r="D6" s="2">
         <v>75.27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>42423</v>
       </c>
@@ -646,8 +699,11 @@
       <c r="D7" s="2">
         <v>90.24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>42459</v>
       </c>
@@ -660,21 +716,67 @@
       <c r="D8" s="2">
         <v>49.35</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" s="3" customFormat="1" ht="38" customHeight="1" thickBot="1">
-      <c r="B21" s="6" t="s">
+      <c r="E8" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>42487</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <v>114.15</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" s="3" customFormat="1" ht="38" customHeight="1" thickBot="1">
+      <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3">
-        <f>SUM(D2:D20)</f>
-        <v>288.54000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="16" thickTop="1"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="3">
+        <f>SUM(D2:D21)</f>
+        <v>402.69000000000005</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
expenses add acrylic sheets and staple gun
</commit_message>
<xml_diff>
--- a/expenses/expenses.xlsx
+++ b/expenses/expenses.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>more power supplies (3)</t>
+  </si>
+  <si>
+    <t>staple gun and staples</t>
+  </si>
+  <si>
+    <t>Tap Plastics</t>
+  </si>
+  <si>
+    <t>6 sheets of acrylic - 4x6 feet</t>
   </si>
 </sst>
 </file>
@@ -191,10 +200,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -252,7 +263,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -272,6 +283,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -291,6 +303,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -620,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -907,29 +920,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:5" s="3" customFormat="1" ht="38" customHeight="1" thickBot="1">
-      <c r="B23" s="9" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>42490</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2">
+        <v>268.5</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>42494</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2">
+        <v>101.93</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="38" customHeight="1" thickBot="1">
+      <c r="B22" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="3">
-        <f>SUM(D2:D22)</f>
-        <v>760</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="2:5" ht="16" thickTop="1"/>
-    <row r="29" spans="2:5">
+      <c r="C22" s="9"/>
+      <c r="D22" s="3">
+        <f>SUM(D2:D21)</f>
+        <v>1130.43</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickTop="1"/>
+    <row r="28" spans="1:5">
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5">
       <c r="D29"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="1:5">
       <c r="D30"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="2:5">
-      <c r="D31"/>
-      <c r="E31"/>
+    <row r="32" spans="1:5">
+      <c r="D32"/>
+      <c r="E32"/>
     </row>
     <row r="33" spans="4:5">
       <c r="D33"/>
@@ -939,13 +990,9 @@
       <c r="D34"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="4:5">
-      <c r="D35"/>
-      <c r="E35"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added chain to expenses
</commit_message>
<xml_diff>
--- a/expenses/expenses.xlsx
+++ b/expenses/expenses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9020" yWindow="940" windowWidth="25500" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>date</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>6 sheets of acrylic - 4x6 feet</t>
+  </si>
+  <si>
+    <t>Chain</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -954,6 +957,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>42494</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2">
+        <v>59.84</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="22" spans="1:5" s="3" customFormat="1" ht="38" customHeight="1" thickBot="1">
       <c r="B22" s="9" t="s">
         <v>14</v>
@@ -961,7 +981,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="3">
         <f>SUM(D2:D21)</f>
-        <v>1130.43</v>
+        <v>1190.27</v>
       </c>
       <c r="E22" s="6"/>
     </row>

</xml_diff>